<commit_message>
Adding logger, testing, configurations
</commit_message>
<xml_diff>
--- a/odm_quote_forecast/anchored_results/NPI PTI & Pega Forecasts.xlsx
+++ b/odm_quote_forecast/anchored_results/NPI PTI & Pega Forecasts.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Forecasts for PEGATRON &amp; PTI TAIWAN" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Forecasts for PEGATRON and PTI TAIWAN" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Program</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>ODM</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Program</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -492,12 +492,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>FAIRVIEW</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -532,12 +532,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>FAIRVIEW</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -572,12 +572,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>FAIRVIEW</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -612,12 +612,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>ADPRRR EE</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
@@ -646,12 +646,12 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>ADPRRR EE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
@@ -680,12 +680,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>ADPRRR EE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
@@ -714,12 +714,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>ADPRRR VE</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -749,21 +749,21 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SBFPF2BV076TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>ADPRRR VE PRQ2</t>
-        </is>
-      </c>
       <c r="E9" t="n">
-        <v>45.35</v>
+        <v>45.39</v>
       </c>
       <c r="F9" t="n">
         <v>202241</v>
@@ -777,10 +777,10 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>45.35000000000001</v>
+        <v>45.39</v>
       </c>
       <c r="J9" t="n">
-        <v>2358.2</v>
+        <v>1815.6</v>
       </c>
     </row>
     <row r="10">
@@ -789,21 +789,21 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>SBFPF2BV153TES1</t>
+          <t>SBFPF2BV076TES1</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>ADPRRR VE PRQ2</t>
-        </is>
-      </c>
       <c r="E10" t="n">
-        <v>45.41</v>
+        <v>45.35</v>
       </c>
       <c r="F10" t="n">
         <v>202241</v>
@@ -817,10 +817,10 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>45.41</v>
+        <v>45.35000000000001</v>
       </c>
       <c r="J10" t="n">
-        <v>7810.52</v>
+        <v>2358.2</v>
       </c>
     </row>
     <row r="11">
@@ -829,21 +829,21 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SBFPF2BV307TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>ADPRRR VE PRQ2</t>
-        </is>
-      </c>
       <c r="E11" t="n">
-        <v>120.88</v>
+        <v>45.41</v>
       </c>
       <c r="F11" t="n">
         <v>202241</v>
@@ -857,10 +857,10 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>120.88</v>
+        <v>45.41</v>
       </c>
       <c r="J11" t="n">
-        <v>12692.4</v>
+        <v>7810.52</v>
       </c>
     </row>
     <row r="12">
@@ -869,20 +869,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SBFPFABU038TES1</t>
+          <t>SBFPF2BV307TES1</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>ADPRRR EE</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>120.88</v>
+      </c>
       <c r="F12" t="n">
         <v>202241</v>
       </c>
@@ -894,8 +896,12 @@
           <t>ACTIVE, WIP, DONE</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
+      <c r="I12" t="n">
+        <v>120.88</v>
+      </c>
+      <c r="J12" t="n">
+        <v>12692.4</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -903,22 +909,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SBFPFABU076TES1</t>
+          <t>SBFPFABU038TES1</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>ADPRRR EE</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>ADPRRR EE</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>53.78</v>
-      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>202241</v>
       </c>
@@ -930,12 +934,8 @@
           <t>ACTIVE, WIP, DONE</t>
         </is>
       </c>
-      <c r="I13" t="n">
-        <v>53.78</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1290.72</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -943,21 +943,21 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SBFPFABU153TES1</t>
+          <t>SBFPFABU076TES1</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>ADPRRR EE</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>ADPRRR EE</t>
-        </is>
-      </c>
       <c r="E14" t="n">
-        <v>53.02</v>
+        <v>53.78</v>
       </c>
       <c r="F14" t="n">
         <v>202241</v>
@@ -971,10 +971,10 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>53.02</v>
+        <v>53.78</v>
       </c>
       <c r="J14" t="n">
-        <v>1060.4</v>
+        <v>1290.72</v>
       </c>
     </row>
     <row r="15">
@@ -983,21 +983,21 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>SBFPFABV076TES1</t>
+          <t>SBFPFABU153TES1</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>ADPRRR EE</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>ADPRRR VE PRQ2</t>
-        </is>
-      </c>
       <c r="E15" t="n">
-        <v>52.96</v>
+        <v>53.02</v>
       </c>
       <c r="F15" t="n">
         <v>202241</v>
@@ -1011,10 +1011,10 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>52.96</v>
+        <v>53.02</v>
       </c>
       <c r="J15" t="n">
-        <v>5084.16</v>
+        <v>1060.4</v>
       </c>
     </row>
     <row r="16">
@@ -1023,21 +1023,21 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SBFPFABV153TES1</t>
+          <t>SBFPFABV076TES1</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>ADPRRR VE PRQ2</t>
-        </is>
-      </c>
       <c r="E16" t="n">
-        <v>53.02</v>
+        <v>52.96</v>
       </c>
       <c r="F16" t="n">
         <v>202241</v>
@@ -1051,10 +1051,10 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>53.02</v>
+        <v>52.96</v>
       </c>
       <c r="J16" t="n">
-        <v>2438.92</v>
+        <v>5084.16</v>
       </c>
     </row>
     <row r="17">
@@ -1063,21 +1063,21 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SBFPFWBV153TES1</t>
+          <t>SBFPFABV153TES1</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>ADPRRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>ADPRRR VE</t>
-        </is>
-      </c>
       <c r="E17" t="n">
-        <v>121.16</v>
+        <v>53.02</v>
       </c>
       <c r="F17" t="n">
         <v>202241</v>
@@ -1091,10 +1091,10 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>121.16</v>
+        <v>53.02</v>
       </c>
       <c r="J17" t="n">
-        <v>13085.28</v>
+        <v>2438.92</v>
       </c>
     </row>
     <row r="18">
@@ -1103,21 +1103,21 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SBFPFWBV307TES1</t>
+          <t>SBFPFWBV153TES1</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>ADPRRR VE</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>ADPRRR VE</t>
-        </is>
-      </c>
       <c r="E18" t="n">
-        <v>120.72</v>
+        <v>121.16</v>
       </c>
       <c r="F18" t="n">
         <v>202241</v>
@@ -1131,10 +1131,10 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>120.72</v>
+        <v>121.16</v>
       </c>
       <c r="J18" t="n">
-        <v>12554.88</v>
+        <v>13085.28</v>
       </c>
     </row>
     <row r="19">
@@ -1143,21 +1143,21 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SSDPF2KX012TZES</t>
+          <t>SBFPFWBV307TES1</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>ADPRRR VE</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>ADPR SE</t>
-        </is>
-      </c>
       <c r="E19" t="n">
-        <v>37.7</v>
+        <v>120.72</v>
       </c>
       <c r="F19" t="n">
         <v>202241</v>
@@ -1171,10 +1171,10 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>37.7</v>
+        <v>120.72</v>
       </c>
       <c r="J19" t="n">
-        <v>2865.2</v>
+        <v>12554.88</v>
       </c>
     </row>
     <row r="20">
@@ -1183,17 +1183,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SSDPF2KX038TZES</t>
+          <t>SSDPF2KX012TZES</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>ADPR SE</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>ADPR SE</t>
         </is>
       </c>
       <c r="E20" t="n">
@@ -1214,7 +1214,7 @@
         <v>37.7</v>
       </c>
       <c r="J20" t="n">
-        <v>6032</v>
+        <v>2865.2</v>
       </c>
     </row>
     <row r="21">
@@ -1223,17 +1223,17 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SSDPF2KX076TZES</t>
+          <t>SSDPF2KX038TZES</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>ADPR SE</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>ADPR SE</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1254,7 +1254,7 @@
         <v>37.7</v>
       </c>
       <c r="J21" t="n">
-        <v>452.4</v>
+        <v>6032</v>
       </c>
     </row>
     <row r="22">
@@ -1263,21 +1263,21 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SSDPFINU512GZ1S</t>
+          <t>SSDPF2KX076TZES</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>ADPR SE</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>EH</t>
-        </is>
-      </c>
       <c r="E22" t="n">
-        <v>5.79</v>
+        <v>37.7</v>
       </c>
       <c r="F22" t="n">
         <v>202241</v>
@@ -1291,10 +1291,10 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>5.79</v>
+        <v>37.7</v>
       </c>
       <c r="J22" t="n">
-        <v>277.92</v>
+        <v>452.4</v>
       </c>
     </row>
     <row r="23">
@@ -1303,17 +1303,17 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SSDPFKNU010TZ1S</t>
+          <t>SSDPFINU512GZ1S</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>EH</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>EH</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1334,7 +1334,7 @@
         <v>5.79</v>
       </c>
       <c r="J23" t="n">
-        <v>555.84</v>
+        <v>277.92</v>
       </c>
     </row>
     <row r="24">
@@ -1343,17 +1343,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SSDPFKNU512GZ1S</t>
+          <t>SSDPFKNU010TZ1S</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>EH</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>EH</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1374,7 +1374,7 @@
         <v>5.79</v>
       </c>
       <c r="J24" t="n">
-        <v>648.48</v>
+        <v>555.84</v>
       </c>
     </row>
     <row r="25">
@@ -1383,21 +1383,21 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PFKNU512GZ</t>
+          <t>SSDPFKNU512GZ1S</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>EH</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PEGATRON</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>45.98</v>
+        <v>5.79</v>
       </c>
       <c r="F25" t="n">
         <v>202241</v>
@@ -1411,10 +1411,10 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>45.98</v>
+        <v>5.79</v>
       </c>
       <c r="J25" t="n">
-        <v>4414.08</v>
+        <v>648.48</v>
       </c>
     </row>
     <row r="26">
@@ -1423,21 +1423,21 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>SBDPFKBP010T</t>
+          <t>PFKNU512GZ</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>FAIRVIEW</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>9.91</v>
+        <v>45.98</v>
       </c>
       <c r="F26" t="n">
         <v>202241</v>
@@ -1451,10 +1451,10 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>9.91</v>
+        <v>45.98</v>
       </c>
       <c r="J26" t="n">
-        <v>356.76</v>
+        <v>4414.08</v>
       </c>
     </row>
     <row r="27">
@@ -1463,21 +1463,21 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SBFPF2BU012TES1</t>
+          <t>SBDPFKBP010T</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>FAIRVIEW</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>38.89090909090909</v>
+        <v>9.91</v>
       </c>
       <c r="F27" t="n">
         <v>202241</v>
@@ -1491,10 +1491,10 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>40.25467532467533</v>
+        <v>9.91</v>
       </c>
       <c r="J27" t="n">
-        <v>3099.454545454545</v>
+        <v>356.76</v>
       </c>
     </row>
     <row r="28">
@@ -1503,21 +1503,21 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>SBFPF2BU038TES1</t>
+          <t>SBFPF2BU012TES1</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>48.2925</v>
+        <v>38.89090909090909</v>
       </c>
       <c r="F28" t="n">
         <v>202241</v>
@@ -1531,10 +1531,10 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>48.3135294117647</v>
+        <v>40.25467532467533</v>
       </c>
       <c r="J28" t="n">
-        <v>4106.65</v>
+        <v>3099.454545454545</v>
       </c>
     </row>
     <row r="29">
@@ -1543,21 +1543,21 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>SBFPF2BU076TES1</t>
+          <t>SBFPF2BU038TES1</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>49.555</v>
+        <v>48.2925</v>
       </c>
       <c r="F29" t="n">
         <v>202241</v>
@@ -1571,10 +1571,10 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>49.59975308641975</v>
+        <v>48.3135294117647</v>
       </c>
       <c r="J29" t="n">
-        <v>4017.58</v>
+        <v>4106.65</v>
       </c>
     </row>
     <row r="30">
@@ -1583,21 +1583,21 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SBFPF2BU153TES1</t>
+          <t>SBFPF2BU076TES1</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>55.515</v>
+        <v>49.555</v>
       </c>
       <c r="F30" t="n">
         <v>202241</v>
@@ -1611,10 +1611,10 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>55.55952380952381</v>
+        <v>49.59975308641975</v>
       </c>
       <c r="J30" t="n">
-        <v>2333.5</v>
+        <v>4017.58</v>
       </c>
     </row>
     <row r="31">
@@ -1623,21 +1623,21 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>SBFPF2BU307TES1</t>
+          <t>SBFPF2BU153TES1</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>106.09</v>
+        <v>55.515</v>
       </c>
       <c r="F31" t="n">
         <v>202241</v>
@@ -1651,10 +1651,10 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>106.0923188405797</v>
+        <v>55.55952380952381</v>
       </c>
       <c r="J31" t="n">
-        <v>5490.2775</v>
+        <v>2333.5</v>
       </c>
     </row>
     <row r="32">
@@ -1663,21 +1663,21 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SBFPF2BV025TES1</t>
+          <t>SBFPF2BU307TES1</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>110.21</v>
+        <v>106.09</v>
       </c>
       <c r="F32" t="n">
         <v>202241</v>
@@ -1691,10 +1691,10 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>56.78142857142858</v>
+        <v>106.0923188405797</v>
       </c>
       <c r="J32" t="n">
-        <v>11806.16</v>
+        <v>5490.2775</v>
       </c>
     </row>
     <row r="33">
@@ -1703,21 +1703,21 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>SBFPF2BV076TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>48.67999999999999</v>
+        <v>48.47</v>
       </c>
       <c r="F33" t="n">
         <v>202241</v>
@@ -1731,10 +1731,10 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>48.67999999999999</v>
+        <v>48.38590163934425</v>
       </c>
       <c r="J33" t="n">
-        <v>4283.839999999999</v>
+        <v>11806.16</v>
       </c>
     </row>
     <row r="34">
@@ -1743,21 +1743,21 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SBFPF2BV153TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>78.21000000000001</v>
+        <v>49.12</v>
       </c>
       <c r="F34" t="n">
         <v>202241</v>
@@ -1771,10 +1771,10 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>78.21000000000001</v>
+        <v>49.12</v>
       </c>
       <c r="J34" t="n">
-        <v>3934.8</v>
+        <v>7073.280000000001</v>
       </c>
     </row>
     <row r="35">
@@ -1783,21 +1783,21 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>SBFPF2BV307TES1</t>
+          <t>SBFPF2BV025TES1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>138.75</v>
+        <v>110.21</v>
       </c>
       <c r="F35" t="n">
         <v>202241</v>
@@ -1811,10 +1811,10 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>138.75</v>
+        <v>56.78142857142858</v>
       </c>
       <c r="J35" t="n">
-        <v>5550</v>
+        <v>2384.82</v>
       </c>
     </row>
     <row r="36">
@@ -1823,21 +1823,21 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>SBFPF2BV614TES1</t>
+          <t>SBFPF2BV076TES1</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>115.555</v>
+        <v>48.67999999999999</v>
       </c>
       <c r="F36" t="n">
         <v>202241</v>
@@ -1851,10 +1851,10 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>116.8689312977099</v>
+        <v>48.67999999999999</v>
       </c>
       <c r="J36" t="n">
-        <v>3827.4575</v>
+        <v>4283.839999999999</v>
       </c>
     </row>
     <row r="37">
@@ -1863,21 +1863,21 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SBFPFABU038TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>60.322</v>
+        <v>55.70000000000001</v>
       </c>
       <c r="F37" t="n">
         <v>202241</v>
@@ -1891,10 +1891,10 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>60.57756756756758</v>
+        <v>55.7</v>
       </c>
       <c r="J37" t="n">
-        <v>1793.096</v>
+        <v>3639.066666666667</v>
       </c>
     </row>
     <row r="38">
@@ -1903,21 +1903,21 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SBFPFABU076TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>60.6</v>
+        <v>54.65</v>
       </c>
       <c r="F38" t="n">
         <v>202241</v>
@@ -1931,10 +1931,10 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>60.9015625</v>
+        <v>54.65</v>
       </c>
       <c r="J38" t="n">
-        <v>2598.466666666667</v>
+        <v>3934.8</v>
       </c>
     </row>
     <row r="39">
@@ -1943,21 +1943,21 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>SBFPFABU153TES1</t>
+          <t>SBFPF2BV153TES1</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>PF</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ADPRRR EE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>61.34</v>
+        <v>78.21000000000001</v>
       </c>
       <c r="F39" t="n">
         <v>202241</v>
@@ -1971,10 +1971,10 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>61.36142857142858</v>
+        <v>78.21000000000001</v>
       </c>
       <c r="J39" t="n">
-        <v>3084.25</v>
+        <v>1877.04</v>
       </c>
     </row>
     <row r="40">
@@ -1983,21 +1983,21 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SBFPFABU307TES1</t>
+          <t>SBFPF2BV307TES1</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>104.495</v>
+        <v>138.75</v>
       </c>
       <c r="F40" t="n">
         <v>202241</v>
@@ -2011,10 +2011,10 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>104.495</v>
+        <v>138.75</v>
       </c>
       <c r="J40" t="n">
-        <v>4806.77</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="41">
@@ -2023,21 +2023,21 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>SBFPFABV076TES1</t>
+          <t>SBFPF2BV614TES1</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>60.66</v>
+        <v>115.555</v>
       </c>
       <c r="F41" t="n">
         <v>202241</v>
@@ -2051,10 +2051,10 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>60.66</v>
+        <v>116.8689312977099</v>
       </c>
       <c r="J41" t="n">
-        <v>485.28</v>
+        <v>3827.4575</v>
       </c>
     </row>
     <row r="42">
@@ -2063,21 +2063,21 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>SBFPFABV153TES1</t>
+          <t>SBFPFABU038TES1</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ4</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>60.13</v>
+        <v>60.322</v>
       </c>
       <c r="F42" t="n">
         <v>202241</v>
@@ -2091,10 +2091,10 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>60.13</v>
+        <v>60.57756756756758</v>
       </c>
       <c r="J42" t="n">
-        <v>1683.64</v>
+        <v>1793.096</v>
       </c>
     </row>
     <row r="43">
@@ -2103,21 +2103,21 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>SBFPFABV307TES1</t>
+          <t>SBFPFABU076TES1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E43" t="n">
-        <v>111.61</v>
+        <v>60.6</v>
       </c>
       <c r="F43" t="n">
         <v>202241</v>
@@ -2131,10 +2131,10 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>114.046</v>
+        <v>60.9015625</v>
       </c>
       <c r="J43" t="n">
-        <v>4561.839999999999</v>
+        <v>2598.466666666667</v>
       </c>
     </row>
     <row r="44">
@@ -2143,21 +2143,21 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>SBFPFUBU038TES1</t>
+          <t>SBFPFABU153TES1</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E44" t="n">
-        <v>66</v>
+        <v>61.34</v>
       </c>
       <c r="F44" t="n">
         <v>202241</v>
@@ -2171,10 +2171,10 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>66</v>
+        <v>61.36142857142858</v>
       </c>
       <c r="J44" t="n">
-        <v>1848</v>
+        <v>3084.25</v>
       </c>
     </row>
     <row r="45">
@@ -2183,21 +2183,21 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>SBFPFUBU076TES1</t>
+          <t>SBFPFABU307TES1</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E45" t="n">
-        <v>65.17</v>
+        <v>104.495</v>
       </c>
       <c r="F45" t="n">
         <v>202241</v>
@@ -2211,10 +2211,10 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>65.16941176470588</v>
+        <v>104.495</v>
       </c>
       <c r="J45" t="n">
-        <v>2215.76</v>
+        <v>4806.77</v>
       </c>
     </row>
     <row r="46">
@@ -2223,21 +2223,21 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>SBFPFUBU153TES1</t>
+          <t>SBFPFABV076TES1</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>ADPRRR EE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>73.4988</v>
+        <v>60.66</v>
       </c>
       <c r="F46" t="n">
         <v>202241</v>
@@ -2251,10 +2251,10 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>85.60758620689654</v>
+        <v>60.66</v>
       </c>
       <c r="J46" t="n">
-        <v>3972.192</v>
+        <v>485.28</v>
       </c>
     </row>
     <row r="47">
@@ -2263,22 +2263,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>SBFPFWBV153TES1</t>
+          <t>SBFPFABV153TES1</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
-        </is>
-      </c>
-      <c r="E47" t="n">
-        <v>98.06</v>
-      </c>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
         <v>202241</v>
       </c>
@@ -2290,12 +2288,8 @@
           <t>ACTIVE, WIP, DONE</t>
         </is>
       </c>
-      <c r="I47" t="n">
-        <v>98.05999999999999</v>
-      </c>
-      <c r="J47" t="n">
-        <v>11704.48</v>
-      </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2303,21 +2297,21 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>SBFPFWBV307TES1</t>
+          <t>SBFPFABV153TES1</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>124.1433333333333</v>
+        <v>60.13</v>
       </c>
       <c r="F48" t="n">
         <v>202241</v>
@@ -2331,10 +2325,10 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>134.7667415730337</v>
+        <v>60.13</v>
       </c>
       <c r="J48" t="n">
-        <v>15992.32</v>
+        <v>1683.64</v>
       </c>
     </row>
     <row r="49">
@@ -2343,21 +2337,21 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>SBFPFWBV614TES1</t>
+          <t>SBFPFABV307TES1</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>ADPRRR VE PRQ2</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>99.88</v>
+        <v>111.61</v>
       </c>
       <c r="F49" t="n">
         <v>202241</v>
@@ -2371,10 +2365,10 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>99.88</v>
+        <v>114.046</v>
       </c>
       <c r="J49" t="n">
-        <v>4661.066666666667</v>
+        <v>4561.839999999999</v>
       </c>
     </row>
     <row r="50">
@@ -2383,21 +2377,21 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>SSDPF2KX012T1ES</t>
+          <t>SBFPFUBU038TES1</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>ADPRR SE (PRQ1)</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E50" t="n">
-        <v>28.114</v>
+        <v>66</v>
       </c>
       <c r="F50" t="n">
         <v>202241</v>
@@ -2411,10 +2405,10 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>28.11482758620689</v>
+        <v>66</v>
       </c>
       <c r="J50" t="n">
-        <v>2609.056</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="51">
@@ -2423,21 +2417,21 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>SSDPF2KX012TZES</t>
+          <t>SBFPFUBU076TES1</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>ADPR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>36.75600000000001</v>
+        <v>65.17</v>
       </c>
       <c r="F51" t="n">
         <v>202241</v>
@@ -2451,10 +2445,10 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>39.26875</v>
+        <v>65.16941176470588</v>
       </c>
       <c r="J51" t="n">
-        <v>3769.8</v>
+        <v>2215.76</v>
       </c>
     </row>
     <row r="52">
@@ -2463,21 +2457,21 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>SSDPF2KX019T1M1</t>
+          <t>SBFPFUBU153TES1</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E52" t="n">
-        <v>42.08</v>
+        <v>73.4988</v>
       </c>
       <c r="F52" t="n">
         <v>202241</v>
@@ -2491,10 +2485,10 @@
         </is>
       </c>
       <c r="I52" t="n">
-        <v>42.08</v>
+        <v>85.60758620689654</v>
       </c>
       <c r="J52" t="n">
-        <v>8416</v>
+        <v>3972.192</v>
       </c>
     </row>
     <row r="53">
@@ -2503,21 +2497,21 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>SSDPF2KX076T1ES</t>
+          <t>SBFPFWBV153TES1</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>ADPRR SE (PRQ1)</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E53" t="n">
-        <v>45.31</v>
+        <v>97.68666666666667</v>
       </c>
       <c r="F53" t="n">
         <v>202241</v>
@@ -2531,10 +2525,10 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>45.31</v>
+        <v>97.53733333333334</v>
       </c>
       <c r="J53" t="n">
-        <v>181.24</v>
+        <v>11704.48</v>
       </c>
     </row>
     <row r="54">
@@ -2543,21 +2537,21 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>SSDPF2KX153T1N1</t>
+          <t>SBFPFWBV153TES1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E54" t="n">
-        <v>104.48</v>
+        <v>98.06</v>
       </c>
       <c r="F54" t="n">
         <v>202241</v>
@@ -2571,10 +2565,10 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>104.48</v>
+        <v>98.05999999999999</v>
       </c>
       <c r="J54" t="n">
-        <v>20896</v>
+        <v>2745.68</v>
       </c>
     </row>
     <row r="55">
@@ -2583,21 +2577,21 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>SSDPF2NV017TZES</t>
+          <t>SBFPFWBV307TES1</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>ADPR VE (PRQ2)</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E55" t="n">
-        <v>26.87</v>
+        <v>124.1433333333333</v>
       </c>
       <c r="F55" t="n">
         <v>202241</v>
@@ -2611,10 +2605,10 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>26.87</v>
+        <v>134.7667415730337</v>
       </c>
       <c r="J55" t="n">
-        <v>2579.52</v>
+        <v>15992.32</v>
       </c>
     </row>
     <row r="56">
@@ -2623,21 +2617,21 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>SSDPFCKE064T1S1</t>
+          <t>SBFPFWBV307TES1</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ADPRR ME (PRQ1)</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E56" t="n">
-        <v>69.96499999999999</v>
+        <v>97.50999999999999</v>
       </c>
       <c r="F56" t="n">
         <v>202241</v>
@@ -2651,10 +2645,10 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>69.96499999999999</v>
+        <v>97.50999999999999</v>
       </c>
       <c r="J56" t="n">
-        <v>13993</v>
+        <v>2340.24</v>
       </c>
     </row>
     <row r="57">
@@ -2663,21 +2657,21 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>SSDPFUKX019T1AP</t>
+          <t>SBFPFWBV614TES1</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E57" t="n">
-        <v>53.06999999999999</v>
+        <v>99.88</v>
       </c>
       <c r="F57" t="n">
         <v>202241</v>
@@ -2691,10 +2685,10 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>53.06999999999999</v>
+        <v>99.88</v>
       </c>
       <c r="J57" t="n">
-        <v>424.5599999999999</v>
+        <v>4661.066666666667</v>
       </c>
     </row>
     <row r="58">
@@ -2703,21 +2697,21 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>SSDPFUKX076T1AP</t>
+          <t>SSDPF2KX012T1ES</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRR SE (PRQ1)</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E58" t="n">
-        <v>58.67</v>
+        <v>28.114</v>
       </c>
       <c r="F58" t="n">
         <v>202241</v>
@@ -2731,10 +2725,10 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>58.67</v>
+        <v>28.11482758620689</v>
       </c>
       <c r="J58" t="n">
-        <v>469.36</v>
+        <v>2609.056</v>
       </c>
     </row>
     <row r="59">
@@ -2743,21 +2737,21 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>SSDPFWKX153T1M2</t>
+          <t>SSDPF2KX012TZES</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPR SE</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>ADPRR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E59" t="n">
-        <v>108.97</v>
+        <v>36.75600000000001</v>
       </c>
       <c r="F59" t="n">
         <v>202241</v>
@@ -2771,10 +2765,10 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>108.97</v>
+        <v>39.26875</v>
       </c>
       <c r="J59" t="n">
-        <v>871.76</v>
+        <v>3769.8</v>
       </c>
     </row>
     <row r="60">
@@ -2783,21 +2777,21 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>SSDPFWKX153T8M2</t>
+          <t>SSDPF2KX019T1M1</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRR SE</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>CDR SE EDSFF</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E60" t="n">
-        <v>104.53</v>
+        <v>42.08</v>
       </c>
       <c r="F60" t="n">
         <v>202241</v>
@@ -2811,10 +2805,10 @@
         </is>
       </c>
       <c r="I60" t="n">
-        <v>104.53</v>
+        <v>42.08</v>
       </c>
       <c r="J60" t="n">
-        <v>1254.36</v>
+        <v>8416</v>
       </c>
     </row>
     <row r="61">
@@ -2823,21 +2817,21 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>SSDPHAKX025TZES</t>
+          <t>SSDPF2KX076T1ES</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRR SE (PRQ1)</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>PF</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E61" t="n">
-        <v>161.56</v>
+        <v>45.31</v>
       </c>
       <c r="F61" t="n">
         <v>202241</v>
@@ -2851,10 +2845,10 @@
         </is>
       </c>
       <c r="I61" t="n">
-        <v>161.56</v>
+        <v>45.31</v>
       </c>
       <c r="J61" t="n">
-        <v>1938.72</v>
+        <v>181.24</v>
       </c>
     </row>
     <row r="62">
@@ -2863,21 +2857,21 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>SSDSC2KB038TZ01</t>
+          <t>SSDPF2KX153T1N1</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPRR SE</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>YV RR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E62" t="n">
-        <v>21.69</v>
+        <v>104.48</v>
       </c>
       <c r="F62" t="n">
         <v>202241</v>
@@ -2891,10 +2885,10 @@
         </is>
       </c>
       <c r="I62" t="n">
-        <v>21.68999999999999</v>
+        <v>104.48</v>
       </c>
       <c r="J62" t="n">
-        <v>2342.52</v>
+        <v>20896</v>
       </c>
     </row>
     <row r="63">
@@ -2903,21 +2897,21 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>SSDSC2KB076TZ01</t>
+          <t>SSDPF2NV017TZES</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PTI TAIWAN</t>
+          <t>ADPR VE (PRQ2)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>YV RR SE</t>
+          <t>PTI TAIWAN</t>
         </is>
       </c>
       <c r="E63" t="n">
-        <v>22.09</v>
+        <v>26.87</v>
       </c>
       <c r="F63" t="n">
         <v>202241</v>
@@ -2931,10 +2925,10 @@
         </is>
       </c>
       <c r="I63" t="n">
-        <v>22.09</v>
+        <v>26.87</v>
       </c>
       <c r="J63" t="n">
-        <v>2076.46</v>
+        <v>2579.52</v>
       </c>
     </row>
     <row r="64">
@@ -2943,37 +2937,357 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>SSDPFCKE064T1S1</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>ADPRR ME (PRQ1)</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>69.96499999999999</v>
+      </c>
+      <c r="F64" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G64" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I64" t="n">
+        <v>69.96499999999999</v>
+      </c>
+      <c r="J64" t="n">
+        <v>13993</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>SSDPFUKX019T1AP</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>53.06999999999999</v>
+      </c>
+      <c r="F65" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G65" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I65" t="n">
+        <v>53.06999999999999</v>
+      </c>
+      <c r="J65" t="n">
+        <v>424.5599999999999</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>SSDPFUKX076T1AP</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>58.67</v>
+      </c>
+      <c r="F66" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G66" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
+        <v>58.67</v>
+      </c>
+      <c r="J66" t="n">
+        <v>469.36</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>SSDPFWKX153T1M2</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>ADPRR SE</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>108.97</v>
+      </c>
+      <c r="F67" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G67" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>108.97</v>
+      </c>
+      <c r="J67" t="n">
+        <v>871.76</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>SSDPFWKX153T8M2</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>CDR SE EDSFF</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>104.53</v>
+      </c>
+      <c r="F68" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G68" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>104.53</v>
+      </c>
+      <c r="J68" t="n">
+        <v>1254.36</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>SSDPHAKX025TZES</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>PF</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>161.56</v>
+      </c>
+      <c r="F69" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G69" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>161.56</v>
+      </c>
+      <c r="J69" t="n">
+        <v>1938.72</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>SSDSC2KB038TZ01</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>YV RR SE</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="F70" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G70" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>21.68999999999999</v>
+      </c>
+      <c r="J70" t="n">
+        <v>2342.52</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>SSDSC2KB076TZ01</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>YV RR SE</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="F71" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G71" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>22.09</v>
+      </c>
+      <c r="J71" t="n">
+        <v>2076.46</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
           <t>SSDSC2KB960GZ01</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>YV RR SE</t>
         </is>
       </c>
-      <c r="E64" t="n">
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
         <v>21.64</v>
       </c>
-      <c r="F64" t="n">
-        <v>202241</v>
-      </c>
-      <c r="G64" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I64" t="n">
+      <c r="F72" t="n">
+        <v>202241</v>
+      </c>
+      <c r="G72" t="n">
+        <v>202253</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="I72" t="n">
         <v>21.64</v>
       </c>
-      <c r="J64" t="n">
+      <c r="J72" t="n">
         <v>2337.12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reading build plan data from SQL db, updating log file, generating new output from VM
</commit_message>
<xml_diff>
--- a/odm_quote_forecast/anchored_results/NPI PTI & Pega Forecasts.xlsx
+++ b/odm_quote_forecast/anchored_results/NPI PTI & Pega Forecasts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:K72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,30 +451,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>Program Acronym</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Forecast for: BOM+MVA Cost (mean)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>WW Start</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>WW End</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Build Status Used</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Forecast for: BOM+MVA Cost (weighted mean)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Forecast for: Subtotal = NRE+
 Qty*(BOM+MVA) (mean)</t>
@@ -492,32 +497,37 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>FAIRVIEW HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>FAIRVIEW</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>5.642222222222221</v>
       </c>
-      <c r="F2" t="n">
-        <v>202241</v>
-      </c>
       <c r="G2" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H2" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
         <v>5.119069767441861</v>
       </c>
-      <c r="J2" t="n">
+      <c r="K2" t="n">
         <v>195.6622222222222</v>
       </c>
     </row>
@@ -532,32 +542,37 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>FAIRVIEW HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>FAIRVIEW</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>5.653999999999999</v>
       </c>
-      <c r="F3" t="n">
-        <v>202241</v>
-      </c>
       <c r="G3" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H3" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
         <v>5.738799999999999</v>
       </c>
-      <c r="J3" t="n">
+      <c r="K3" t="n">
         <v>229.552</v>
       </c>
     </row>
@@ -572,32 +587,37 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>FAIRVIEW HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>FAIRVIEW</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>5.642222222222221</v>
       </c>
-      <c r="F4" t="n">
-        <v>202241</v>
-      </c>
       <c r="G4" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H4" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
         <v>5.270769230769229</v>
       </c>
-      <c r="J4" t="n">
+      <c r="K4" t="n">
         <v>304.5333333333332</v>
       </c>
     </row>
@@ -612,28 +632,33 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>202241</v>
-      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr"/>
+        <v>202241</v>
+      </c>
+      <c r="H5" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -646,28 +671,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="n">
-        <v>202241</v>
-      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr"/>
+        <v>202241</v>
+      </c>
+      <c r="H6" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -680,28 +710,33 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="n">
-        <v>202241</v>
-      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr"/>
+        <v>202241</v>
+      </c>
+      <c r="H7" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
       <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -714,32 +749,37 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>ADPRRR VE</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>45.39</v>
       </c>
-      <c r="F8" t="n">
-        <v>202241</v>
-      </c>
       <c r="G8" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H8" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
         <v>45.39</v>
       </c>
-      <c r="J8" t="n">
+      <c r="K8" t="n">
         <v>6354.6</v>
       </c>
     </row>
@@ -754,32 +794,37 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>45.39</v>
       </c>
-      <c r="F9" t="n">
-        <v>202241</v>
-      </c>
       <c r="G9" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H9" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
         <v>45.39</v>
       </c>
-      <c r="J9" t="n">
+      <c r="K9" t="n">
         <v>1815.6</v>
       </c>
     </row>
@@ -794,32 +839,37 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>45.35</v>
       </c>
-      <c r="F10" t="n">
-        <v>202241</v>
-      </c>
       <c r="G10" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H10" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
         <v>45.35000000000001</v>
       </c>
-      <c r="J10" t="n">
+      <c r="K10" t="n">
         <v>2358.2</v>
       </c>
     </row>
@@ -834,32 +884,37 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>45.41</v>
       </c>
-      <c r="F11" t="n">
-        <v>202241</v>
-      </c>
       <c r="G11" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H11" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
         <v>45.41</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>7810.52</v>
       </c>
     </row>
@@ -874,32 +929,37 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>120.88</v>
       </c>
-      <c r="F12" t="n">
-        <v>202241</v>
-      </c>
       <c r="G12" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H12" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
         <v>120.88</v>
       </c>
-      <c r="J12" t="n">
+      <c r="K12" t="n">
         <v>12692.4</v>
       </c>
     </row>
@@ -914,28 +974,33 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>202241</v>
-      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr"/>
+        <v>202241</v>
+      </c>
+      <c r="H13" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -948,32 +1013,37 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>53.78</v>
       </c>
-      <c r="F14" t="n">
-        <v>202241</v>
-      </c>
       <c r="G14" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H14" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
         <v>53.78</v>
       </c>
-      <c r="J14" t="n">
+      <c r="K14" t="n">
         <v>1290.72</v>
       </c>
     </row>
@@ -988,32 +1058,37 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>53.02</v>
       </c>
-      <c r="F15" t="n">
-        <v>202241</v>
-      </c>
       <c r="G15" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H15" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
         <v>53.02</v>
       </c>
-      <c r="J15" t="n">
+      <c r="K15" t="n">
         <v>1060.4</v>
       </c>
     </row>
@@ -1028,32 +1103,37 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>52.96</v>
       </c>
-      <c r="F16" t="n">
-        <v>202241</v>
-      </c>
       <c r="G16" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H16" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
         <v>52.96</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>5084.16</v>
       </c>
     </row>
@@ -1068,32 +1148,37 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>53.02</v>
       </c>
-      <c r="F17" t="n">
-        <v>202241</v>
-      </c>
       <c r="G17" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H17" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
         <v>53.02</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>2438.92</v>
       </c>
     </row>
@@ -1108,32 +1193,37 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
           <t>ADPRRR VE</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>121.16</v>
       </c>
-      <c r="F18" t="n">
-        <v>202241</v>
-      </c>
       <c r="G18" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H18" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
         <v>121.16</v>
       </c>
-      <c r="J18" t="n">
+      <c r="K18" t="n">
         <v>13085.28</v>
       </c>
     </row>
@@ -1148,32 +1238,37 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
           <t>ADPRRR VE</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>120.72</v>
       </c>
-      <c r="F19" t="n">
-        <v>202241</v>
-      </c>
       <c r="G19" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H19" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
         <v>120.72</v>
       </c>
-      <c r="J19" t="n">
+      <c r="K19" t="n">
         <v>12554.88</v>
       </c>
     </row>
@@ -1188,32 +1283,37 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS R SE PRQ1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
           <t>ADPR SE</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>37.7</v>
       </c>
-      <c r="F20" t="n">
-        <v>202241</v>
-      </c>
       <c r="G20" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H20" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
         <v>37.7</v>
       </c>
-      <c r="J20" t="n">
+      <c r="K20" t="n">
         <v>2865.2</v>
       </c>
     </row>
@@ -1228,32 +1328,37 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS R SE PRQ1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
           <t>ADPR SE</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>37.7</v>
       </c>
-      <c r="F21" t="n">
-        <v>202241</v>
-      </c>
       <c r="G21" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H21" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
         <v>37.7</v>
       </c>
-      <c r="J21" t="n">
+      <c r="K21" t="n">
         <v>6032</v>
       </c>
     </row>
@@ -1268,32 +1373,37 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS R SE PRQ1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
           <t>ADPR SE</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>37.7</v>
       </c>
-      <c r="F22" t="n">
-        <v>202241</v>
-      </c>
       <c r="G22" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H22" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
         <v>37.7</v>
       </c>
-      <c r="J22" t="n">
+      <c r="K22" t="n">
         <v>452.4</v>
       </c>
     </row>
@@ -1308,32 +1418,37 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>ECHO HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
           <t>EH</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>5.79</v>
       </c>
-      <c r="F23" t="n">
-        <v>202241</v>
-      </c>
       <c r="G23" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H23" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
         <v>5.79</v>
       </c>
-      <c r="J23" t="n">
+      <c r="K23" t="n">
         <v>277.92</v>
       </c>
     </row>
@@ -1348,32 +1463,37 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>ECHO HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
           <t>EH</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>5.79</v>
       </c>
-      <c r="F24" t="n">
-        <v>202241</v>
-      </c>
       <c r="G24" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H24" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
         <v>5.79</v>
       </c>
-      <c r="J24" t="n">
+      <c r="K24" t="n">
         <v>555.84</v>
       </c>
     </row>
@@ -1388,32 +1508,37 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>ECHO HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>PEGATRON</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
           <t>EH</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>PEGATRON</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>5.79</v>
       </c>
-      <c r="F25" t="n">
-        <v>202241</v>
-      </c>
       <c r="G25" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H25" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
         <v>5.79</v>
       </c>
-      <c r="J25" t="n">
+      <c r="K25" t="n">
         <v>648.48</v>
       </c>
     </row>
@@ -1428,32 +1553,37 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
+      <c r="F26" t="n">
         <v>45.98</v>
       </c>
-      <c r="F26" t="n">
-        <v>202241</v>
-      </c>
       <c r="G26" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I26" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H26" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
         <v>45.98</v>
       </c>
-      <c r="J26" t="n">
+      <c r="K26" t="n">
         <v>4414.08</v>
       </c>
     </row>
@@ -1468,32 +1598,37 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t>FAIRVIEW HARBOR PRQ1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
           <t>FAIRVIEW</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>9.91</v>
       </c>
-      <c r="F27" t="n">
-        <v>202241</v>
-      </c>
       <c r="G27" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H27" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
         <v>9.91</v>
       </c>
-      <c r="J27" t="n">
+      <c r="K27" t="n">
         <v>356.76</v>
       </c>
     </row>
@@ -1508,32 +1643,37 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>38.89090909090909</v>
       </c>
-      <c r="F28" t="n">
-        <v>202241</v>
-      </c>
       <c r="G28" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I28" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H28" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
         <v>40.25467532467533</v>
       </c>
-      <c r="J28" t="n">
+      <c r="K28" t="n">
         <v>3099.454545454545</v>
       </c>
     </row>
@@ -1548,32 +1688,37 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>48.2925</v>
       </c>
-      <c r="F29" t="n">
-        <v>202241</v>
-      </c>
       <c r="G29" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I29" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H29" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
         <v>48.3135294117647</v>
       </c>
-      <c r="J29" t="n">
+      <c r="K29" t="n">
         <v>4106.65</v>
       </c>
     </row>
@@ -1588,32 +1733,37 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>49.555</v>
       </c>
-      <c r="F30" t="n">
-        <v>202241</v>
-      </c>
       <c r="G30" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I30" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H30" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
         <v>49.59975308641975</v>
       </c>
-      <c r="J30" t="n">
+      <c r="K30" t="n">
         <v>4017.58</v>
       </c>
     </row>
@@ -1628,32 +1778,37 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>55.515</v>
       </c>
-      <c r="F31" t="n">
-        <v>202241</v>
-      </c>
       <c r="G31" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I31" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H31" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
         <v>55.55952380952381</v>
       </c>
-      <c r="J31" t="n">
+      <c r="K31" t="n">
         <v>2333.5</v>
       </c>
     </row>
@@ -1668,32 +1823,37 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
           <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>106.09</v>
       </c>
-      <c r="F32" t="n">
-        <v>202241</v>
-      </c>
       <c r="G32" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H32" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
         <v>106.0923188405797</v>
       </c>
-      <c r="J32" t="n">
+      <c r="K32" t="n">
         <v>5490.2775</v>
       </c>
     </row>
@@ -1708,32 +1868,37 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
           <t>ADPRRR VE</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>48.47</v>
       </c>
-      <c r="F33" t="n">
-        <v>202241</v>
-      </c>
       <c r="G33" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H33" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
         <v>48.38590163934425</v>
       </c>
-      <c r="J33" t="n">
+      <c r="K33" t="n">
         <v>11806.16</v>
       </c>
     </row>
@@ -1748,32 +1913,37 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>49.12</v>
       </c>
-      <c r="F34" t="n">
-        <v>202241</v>
-      </c>
       <c r="G34" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H34" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
         <v>49.12</v>
       </c>
-      <c r="J34" t="n">
+      <c r="K34" t="n">
         <v>7073.280000000001</v>
       </c>
     </row>
@@ -1788,32 +1958,37 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>110.21</v>
       </c>
-      <c r="F35" t="n">
-        <v>202241</v>
-      </c>
       <c r="G35" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H35" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
         <v>56.78142857142858</v>
       </c>
-      <c r="J35" t="n">
+      <c r="K35" t="n">
         <v>2384.82</v>
       </c>
     </row>
@@ -1828,32 +2003,37 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>48.67999999999999</v>
       </c>
-      <c r="F36" t="n">
-        <v>202241</v>
-      </c>
       <c r="G36" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H36" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
         <v>48.67999999999999</v>
       </c>
-      <c r="J36" t="n">
+      <c r="K36" t="n">
         <v>4283.839999999999</v>
       </c>
     </row>
@@ -1868,32 +2048,37 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>55.70000000000001</v>
       </c>
-      <c r="F37" t="n">
-        <v>202241</v>
-      </c>
       <c r="G37" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I37" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H37" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
         <v>55.7</v>
       </c>
-      <c r="J37" t="n">
+      <c r="K37" t="n">
         <v>3639.066666666667</v>
       </c>
     </row>
@@ -1908,32 +2093,37 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>54.65</v>
       </c>
-      <c r="F38" t="n">
-        <v>202241</v>
-      </c>
       <c r="G38" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I38" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H38" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
         <v>54.65</v>
       </c>
-      <c r="J38" t="n">
+      <c r="K38" t="n">
         <v>3934.8</v>
       </c>
     </row>
@@ -1948,32 +2138,37 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>78.21000000000001</v>
       </c>
-      <c r="F39" t="n">
-        <v>202241</v>
-      </c>
       <c r="G39" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H39" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
         <v>78.21000000000001</v>
       </c>
-      <c r="J39" t="n">
+      <c r="K39" t="n">
         <v>1877.04</v>
       </c>
     </row>
@@ -1988,32 +2183,37 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>138.75</v>
       </c>
-      <c r="F40" t="n">
-        <v>202241</v>
-      </c>
       <c r="G40" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I40" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H40" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
         <v>138.75</v>
       </c>
-      <c r="J40" t="n">
+      <c r="K40" t="n">
         <v>5550</v>
       </c>
     </row>
@@ -2028,32 +2228,37 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>115.555</v>
       </c>
-      <c r="F41" t="n">
-        <v>202241</v>
-      </c>
       <c r="G41" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H41" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
         <v>116.8689312977099</v>
       </c>
-      <c r="J41" t="n">
+      <c r="K41" t="n">
         <v>3827.4575</v>
       </c>
     </row>
@@ -2068,32 +2273,37 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>60.322</v>
       </c>
-      <c r="F42" t="n">
-        <v>202241</v>
-      </c>
       <c r="G42" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H42" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
         <v>60.57756756756758</v>
       </c>
-      <c r="J42" t="n">
+      <c r="K42" t="n">
         <v>1793.096</v>
       </c>
     </row>
@@ -2108,32 +2318,37 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>60.6</v>
       </c>
-      <c r="F43" t="n">
-        <v>202241</v>
-      </c>
       <c r="G43" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I43" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H43" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
         <v>60.9015625</v>
       </c>
-      <c r="J43" t="n">
+      <c r="K43" t="n">
         <v>2598.466666666667</v>
       </c>
     </row>
@@ -2148,32 +2363,37 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ1</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
           <t>ADPRRR EE</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>61.34</v>
       </c>
-      <c r="F44" t="n">
-        <v>202241</v>
-      </c>
       <c r="G44" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I44" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H44" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
         <v>61.36142857142858</v>
       </c>
-      <c r="J44" t="n">
+      <c r="K44" t="n">
         <v>3084.25</v>
       </c>
     </row>
@@ -2188,32 +2408,37 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
           <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>104.495</v>
       </c>
-      <c r="F45" t="n">
-        <v>202241</v>
-      </c>
       <c r="G45" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H45" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
         <v>104.495</v>
       </c>
-      <c r="J45" t="n">
+      <c r="K45" t="n">
         <v>4806.77</v>
       </c>
     </row>
@@ -2228,32 +2453,37 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>60.66</v>
       </c>
-      <c r="F46" t="n">
-        <v>202241</v>
-      </c>
       <c r="G46" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I46" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H46" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
         <v>60.66</v>
       </c>
-      <c r="J46" t="n">
+      <c r="K46" t="n">
         <v>485.28</v>
       </c>
     </row>
@@ -2268,28 +2498,33 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="n">
-        <v>202241</v>
-      </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I47" t="inlineStr"/>
+        <v>202241</v>
+      </c>
+      <c r="H47" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
       <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2302,32 +2537,37 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ4</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ4</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>60.13</v>
       </c>
-      <c r="F48" t="n">
-        <v>202241</v>
-      </c>
       <c r="G48" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I48" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H48" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
         <v>60.13</v>
       </c>
-      <c r="J48" t="n">
+      <c r="K48" t="n">
         <v>1683.64</v>
       </c>
     </row>
@@ -2342,32 +2582,37 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>111.61</v>
       </c>
-      <c r="F49" t="n">
-        <v>202241</v>
-      </c>
       <c r="G49" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I49" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H49" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J49" t="n">
         <v>114.046</v>
       </c>
-      <c r="J49" t="n">
+      <c r="K49" t="n">
         <v>4561.839999999999</v>
       </c>
     </row>
@@ -2382,32 +2627,37 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
           <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>66</v>
       </c>
-      <c r="F50" t="n">
-        <v>202241</v>
-      </c>
       <c r="G50" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I50" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H50" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J50" t="n">
         <v>66</v>
       </c>
-      <c r="J50" t="n">
+      <c r="K50" t="n">
         <v>1848</v>
       </c>
     </row>
@@ -2422,32 +2672,37 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
           <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>65.17</v>
       </c>
-      <c r="F51" t="n">
-        <v>202241</v>
-      </c>
       <c r="G51" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I51" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H51" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J51" t="n">
         <v>65.16941176470588</v>
       </c>
-      <c r="J51" t="n">
+      <c r="K51" t="n">
         <v>2215.76</v>
       </c>
     </row>
@@ -2462,32 +2717,37 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR EE PRQ2</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
           <t>ADPRRR EE PRQ2</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>73.4988</v>
       </c>
-      <c r="F52" t="n">
-        <v>202241</v>
-      </c>
       <c r="G52" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I52" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H52" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J52" t="n">
         <v>85.60758620689654</v>
       </c>
-      <c r="J52" t="n">
+      <c r="K52" t="n">
         <v>3972.192</v>
       </c>
     </row>
@@ -2502,32 +2762,37 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
           <t>ADPRRR VE</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
         <v>97.68666666666667</v>
       </c>
-      <c r="F53" t="n">
-        <v>202241</v>
-      </c>
       <c r="G53" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I53" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H53" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J53" t="n">
         <v>97.53733333333334</v>
       </c>
-      <c r="J53" t="n">
+      <c r="K53" t="n">
         <v>11704.48</v>
       </c>
     </row>
@@ -2542,32 +2807,37 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
         <v>98.06</v>
       </c>
-      <c r="F54" t="n">
-        <v>202241</v>
-      </c>
       <c r="G54" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I54" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H54" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J54" t="n">
         <v>98.05999999999999</v>
       </c>
-      <c r="J54" t="n">
+      <c r="K54" t="n">
         <v>2745.68</v>
       </c>
     </row>
@@ -2582,32 +2852,37 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ1</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
           <t>ADPRRR VE</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>124.1433333333333</v>
       </c>
-      <c r="F55" t="n">
-        <v>202241</v>
-      </c>
       <c r="G55" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I55" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H55" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J55" t="n">
         <v>134.7667415730337</v>
       </c>
-      <c r="J55" t="n">
+      <c r="K55" t="n">
         <v>15992.32</v>
       </c>
     </row>
@@ -2622,32 +2897,37 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
         <v>97.50999999999999</v>
       </c>
-      <c r="F56" t="n">
-        <v>202241</v>
-      </c>
       <c r="G56" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I56" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H56" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J56" t="n">
         <v>97.50999999999999</v>
       </c>
-      <c r="J56" t="n">
+      <c r="K56" t="n">
         <v>2340.24</v>
       </c>
     </row>
@@ -2662,32 +2942,37 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RRR VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
           <t>ADPRRR VE PRQ2</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
         <v>99.88</v>
       </c>
-      <c r="F57" t="n">
-        <v>202241</v>
-      </c>
       <c r="G57" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I57" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H57" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J57" t="n">
         <v>99.88</v>
       </c>
-      <c r="J57" t="n">
+      <c r="K57" t="n">
         <v>4661.066666666667</v>
       </c>
     </row>
@@ -2702,32 +2987,37 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE PRQ1</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
           <t>ADPRR SE (PRQ1)</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>28.114</v>
       </c>
-      <c r="F58" t="n">
-        <v>202241</v>
-      </c>
       <c r="G58" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H58" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J58" t="n">
         <v>28.11482758620689</v>
       </c>
-      <c r="J58" t="n">
+      <c r="K58" t="n">
         <v>2609.056</v>
       </c>
     </row>
@@ -2742,32 +3032,37 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS R SE PRQ1</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
           <t>ADPR SE</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>36.75600000000001</v>
       </c>
-      <c r="F59" t="n">
-        <v>202241</v>
-      </c>
       <c r="G59" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I59" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H59" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J59" t="n">
         <v>39.26875</v>
       </c>
-      <c r="J59" t="n">
+      <c r="K59" t="n">
         <v>3769.8</v>
       </c>
     </row>
@@ -2782,32 +3077,37 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
           <t>ADPRR SE</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E60" t="n">
+      <c r="F60" t="n">
         <v>42.08</v>
       </c>
-      <c r="F60" t="n">
-        <v>202241</v>
-      </c>
       <c r="G60" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I60" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H60" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J60" t="n">
         <v>42.08</v>
       </c>
-      <c r="J60" t="n">
+      <c r="K60" t="n">
         <v>8416</v>
       </c>
     </row>
@@ -2822,32 +3122,37 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE PRQ1</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
           <t>ADPRR SE (PRQ1)</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
         <v>45.31</v>
       </c>
-      <c r="F61" t="n">
-        <v>202241</v>
-      </c>
       <c r="G61" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I61" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H61" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J61" t="n">
         <v>45.31</v>
       </c>
-      <c r="J61" t="n">
+      <c r="K61" t="n">
         <v>181.24</v>
       </c>
     </row>
@@ -2862,32 +3167,37 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
           <t>ADPRR SE</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
         <v>104.48</v>
       </c>
-      <c r="F62" t="n">
-        <v>202241</v>
-      </c>
       <c r="G62" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I62" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H62" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J62" t="n">
         <v>104.48</v>
       </c>
-      <c r="J62" t="n">
+      <c r="K62" t="n">
         <v>20896</v>
       </c>
     </row>
@@ -2902,32 +3212,37 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS R VE PRQ2</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
           <t>ADPR VE (PRQ2)</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>26.87</v>
       </c>
-      <c r="F63" t="n">
-        <v>202241</v>
-      </c>
       <c r="G63" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I63" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H63" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J63" t="n">
         <v>26.87</v>
       </c>
-      <c r="J63" t="n">
+      <c r="K63" t="n">
         <v>2579.52</v>
       </c>
     </row>
@@ -2942,32 +3257,37 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR ME</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
           <t>ADPRR ME (PRQ1)</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>69.96499999999999</v>
       </c>
-      <c r="F64" t="n">
-        <v>202241</v>
-      </c>
       <c r="G64" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I64" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H64" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J64" t="n">
         <v>69.96499999999999</v>
       </c>
-      <c r="J64" t="n">
+      <c r="K64" t="n">
         <v>13993</v>
       </c>
     </row>
@@ -2982,32 +3302,37 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
           <t>ADPRR SE</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>53.06999999999999</v>
       </c>
-      <c r="F65" t="n">
-        <v>202241</v>
-      </c>
       <c r="G65" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I65" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H65" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J65" t="n">
         <v>53.06999999999999</v>
       </c>
-      <c r="J65" t="n">
+      <c r="K65" t="n">
         <v>424.5599999999999</v>
       </c>
     </row>
@@ -3022,32 +3347,37 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
           <t>ADPRR SE</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E66" t="n">
+      <c r="F66" t="n">
         <v>58.67</v>
       </c>
-      <c r="F66" t="n">
-        <v>202241</v>
-      </c>
       <c r="G66" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H66" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J66" t="n">
         <v>58.67</v>
       </c>
-      <c r="J66" t="n">
+      <c r="K66" t="n">
         <v>469.36</v>
       </c>
     </row>
@@ -3062,32 +3392,37 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t>ARBORDALE PLUS RR SE</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
           <t>ADPRR SE</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
         <v>108.97</v>
       </c>
-      <c r="F67" t="n">
-        <v>202241</v>
-      </c>
       <c r="G67" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I67" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H67" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J67" t="n">
         <v>108.97</v>
       </c>
-      <c r="J67" t="n">
+      <c r="K67" t="n">
         <v>871.76</v>
       </c>
     </row>
@@ -3110,24 +3445,29 @@
           <t>PTI TAIWAN</t>
         </is>
       </c>
-      <c r="E68" t="n">
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>CDR SE EDSFF</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
         <v>104.53</v>
       </c>
-      <c r="F68" t="n">
-        <v>202241</v>
-      </c>
       <c r="G68" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I68" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H68" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J68" t="n">
         <v>104.53</v>
       </c>
-      <c r="J68" t="n">
+      <c r="K68" t="n">
         <v>1254.36</v>
       </c>
     </row>
@@ -3142,32 +3482,37 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
+          <t>NPSG PATHFINDING</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
           <t>PF</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E69" t="n">
+      <c r="F69" t="n">
         <v>161.56</v>
       </c>
-      <c r="F69" t="n">
-        <v>202241</v>
-      </c>
       <c r="G69" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H69" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J69" t="n">
         <v>161.56</v>
       </c>
-      <c r="J69" t="n">
+      <c r="K69" t="n">
         <v>1938.72</v>
       </c>
     </row>
@@ -3182,32 +3527,37 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
+          <t>YOUNGSVILLE RR SE</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
           <t>YV RR SE</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E70" t="n">
+      <c r="F70" t="n">
         <v>21.69</v>
       </c>
-      <c r="F70" t="n">
-        <v>202241</v>
-      </c>
       <c r="G70" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I70" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H70" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J70" t="n">
         <v>21.68999999999999</v>
       </c>
-      <c r="J70" t="n">
+      <c r="K70" t="n">
         <v>2342.52</v>
       </c>
     </row>
@@ -3222,32 +3572,37 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
+          <t>YOUNGSVILLE RR SE</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
           <t>YV RR SE</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E71" t="n">
+      <c r="F71" t="n">
         <v>22.09</v>
       </c>
-      <c r="F71" t="n">
-        <v>202241</v>
-      </c>
       <c r="G71" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I71" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H71" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J71" t="n">
         <v>22.09</v>
       </c>
-      <c r="J71" t="n">
+      <c r="K71" t="n">
         <v>2076.46</v>
       </c>
     </row>
@@ -3262,32 +3617,37 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t>YOUNGSVILLE RR SE</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>PTI TAIWAN</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
           <t>YV RR SE</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>PTI TAIWAN</t>
-        </is>
-      </c>
-      <c r="E72" t="n">
+      <c r="F72" t="n">
         <v>21.64</v>
       </c>
-      <c r="F72" t="n">
-        <v>202241</v>
-      </c>
       <c r="G72" t="n">
-        <v>202253</v>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>ACTIVE, WIP, DONE</t>
-        </is>
-      </c>
-      <c r="I72" t="n">
+        <v>202241</v>
+      </c>
+      <c r="H72" t="n">
+        <v>202253</v>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>ACTIVE, WIP, DONE</t>
+        </is>
+      </c>
+      <c r="J72" t="n">
         <v>21.64</v>
       </c>
-      <c r="J72" t="n">
+      <c r="K72" t="n">
         <v>2337.12</v>
       </c>
     </row>

</xml_diff>